<commit_message>
Comprehensive testing completed - fix verified for all edge cases
Co-authored-by: vamshi620 <27879038+vamshi620@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/test_output/Add_Records.xlsx
+++ b/test_output/Add_Records.xlsx
@@ -16,6 +16,9 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:si>
+    <x:t>Employee_ID</x:t>
+  </x:si>
+  <x:si>
     <x:t>Name</x:t>
   </x:si>
   <x:si>
@@ -31,6 +34,9 @@
     <x:t>Predicted Category</x:t>
   </x:si>
   <x:si>
+    <x:t>001</x:t>
+  </x:si>
+  <x:si>
     <x:t>John Doe</x:t>
   </x:si>
   <x:si>
@@ -44,6 +50,9 @@
   </x:si>
   <x:si>
     <x:t>Add</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Eve Adams</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -409,20 +418,21 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:E2"/>
+  <x:dimension ref="A1:F3"/>
   <x:sheetViews>
     <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="15"/>
   <x:cols>
-    <x:col min="1" max="1" width="9.282054" style="0" customWidth="1"/>
-    <x:col min="2" max="2" width="19.139196" style="0" customWidth="1"/>
-    <x:col min="3" max="3" width="11.710625" style="0" customWidth="1"/>
-    <x:col min="4" max="4" width="27.567768" style="0" customWidth="1"/>
-    <x:col min="5" max="5" width="18.139196" style="0" customWidth="1"/>
+    <x:col min="1" max="1" width="12.853482" style="0" customWidth="1"/>
+    <x:col min="2" max="2" width="10.567768" style="0" customWidth="1"/>
+    <x:col min="3" max="3" width="19.139196" style="0" customWidth="1"/>
+    <x:col min="4" max="4" width="11.710625" style="0" customWidth="1"/>
+    <x:col min="5" max="5" width="27.567768" style="0" customWidth="1"/>
+    <x:col min="6" max="6" width="18.139196" style="0" customWidth="1"/>
   </x:cols>
   <x:sheetData>
-    <x:row r="1" spans="1:5">
+    <x:row r="1" spans="1:6">
       <x:c r="A1" s="1" t="s">
         <x:v>0</x:v>
       </x:c>
@@ -438,22 +448,36 @@
       <x:c r="E1" s="1" t="s">
         <x:v>4</x:v>
       </x:c>
+      <x:c r="F1" s="1" t="s">
+        <x:v>5</x:v>
+      </x:c>
     </x:row>
-    <x:row r="2" spans="1:5">
+    <x:row r="2" spans="1:6">
       <x:c r="A2" s="0" t="s">
-        <x:v>5</x:v>
+        <x:v>6</x:v>
       </x:c>
       <x:c r="B2" s="0" t="s">
-        <x:v>6</x:v>
+        <x:v>7</x:v>
       </x:c>
       <x:c r="C2" s="0" t="s">
-        <x:v>7</x:v>
+        <x:v>8</x:v>
       </x:c>
       <x:c r="D2" s="0" t="s">
-        <x:v>8</x:v>
+        <x:v>9</x:v>
       </x:c>
       <x:c r="E2" s="0" t="s">
-        <x:v>9</x:v>
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="F2" s="0" t="s">
+        <x:v>11</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="3" spans="1:6">
+      <x:c r="B3" s="0" t="s">
+        <x:v>12</x:v>
+      </x:c>
+      <x:c r="F3" s="0" t="s">
+        <x:v>11</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>